<commit_message>
Experiments.R code cleared / Add plot_increasing_pressures.R FUNCTION / Add interaction matrix with autoregulation on cultural and supporting services for hidden-pattern interpretation
</commit_message>
<xml_diff>
--- a/METADATA.xlsx
+++ b/METADATA.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avala\OneDrive\Documents\Cours ACO\M2\Stage M2\IMR Tromsö\Qualitative models\Data\R\Comparison QM_FCM\Qualitative-Modeling-BarentsRISK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3CA079-BE7A-487B-9CD2-97B37EBF55E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A142113-F2B5-48F7-AE72-7E6AF559C785}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{DE23FC9B-3A8E-4A4A-A6E5-7A2ABE12ED8E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{DE23FC9B-3A8E-4A4A-A6E5-7A2ABE12ED8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
     <sheet name="Scenarios" sheetId="3" r:id="rId2"/>
-    <sheet name="No_autoregulation" sheetId="2" r:id="rId3"/>
+    <sheet name="Scenarios_Increasing_Pressures" sheetId="4" r:id="rId3"/>
+    <sheet name="No_autoregulation" sheetId="2" r:id="rId4"/>
+    <sheet name="Auto_regul_cult_sup_serv" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="39">
   <si>
     <t>Marine Transport</t>
   </si>
@@ -174,12 +176,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="11">
@@ -308,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -344,6 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,10 +710,934 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8CA224-94F0-4CBF-A08D-EE426145B91A}">
+  <dimension ref="B1:R18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+    </row>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>-1</v>
+      </c>
+      <c r="I4">
+        <v>-1</v>
+      </c>
+      <c r="J4">
+        <v>-1</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>-1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>-1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>-1</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>-1</v>
+      </c>
+      <c r="Q11">
+        <v>-1</v>
+      </c>
+      <c r="R11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>-1</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>-1</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>-1</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44D56227-A753-4FEA-960B-AC36DE70A80C}">
   <dimension ref="B2:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,24 +1676,12 @@
       <c r="L2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B3">
@@ -796,76 +1717,40 @@
       <c r="L3">
         <v>0</v>
       </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H4">
-        <v>-1</v>
+        <v>0.6</v>
       </c>
       <c r="I4">
-        <v>-1</v>
+        <v>0.7</v>
       </c>
       <c r="J4">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
@@ -873,51 +1758,33 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
         <v>0</v>
       </c>
     </row>
@@ -955,24 +1822,6 @@
       <c r="L6">
         <v>0</v>
       </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7">
@@ -1008,24 +1857,6 @@
       <c r="L7">
         <v>0</v>
       </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8">
@@ -1061,24 +1892,6 @@
       <c r="L8">
         <v>0</v>
       </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9">
@@ -1114,24 +1927,6 @@
       <c r="L9">
         <v>0</v>
       </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10">
@@ -1167,24 +1962,6 @@
       <c r="L10">
         <v>0</v>
       </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B11">
@@ -1215,28 +1992,10 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11">
-        <v>1</v>
-      </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>-1</v>
-      </c>
-      <c r="Q11">
-        <v>-1</v>
-      </c>
-      <c r="R11">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
@@ -1273,24 +2032,6 @@
       <c r="L12">
         <v>0</v>
       </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-      <c r="R12">
-        <v>0</v>
-      </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B13">
@@ -1321,28 +2062,10 @@
         <v>0</v>
       </c>
       <c r="K13">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="L13">
         <v>0</v>
-      </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
-      <c r="N13">
-        <v>-1</v>
-      </c>
-      <c r="O13">
-        <v>1</v>
-      </c>
-      <c r="P13">
-        <v>-1</v>
-      </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-      <c r="R13">
-        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.3">
@@ -1379,24 +2102,6 @@
       <c r="L14">
         <v>0</v>
       </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
-      <c r="R14">
-        <v>0</v>
-      </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B15">
@@ -1432,24 +2137,6 @@
       <c r="L15">
         <v>0</v>
       </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
-      <c r="R15">
-        <v>0</v>
-      </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B16">
@@ -1485,26 +2172,8 @@
       <c r="L16">
         <v>0</v>
       </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="R16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>0</v>
       </c>
@@ -1538,26 +2207,8 @@
       <c r="L17">
         <v>0</v>
       </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-      <c r="R17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>0</v>
       </c>
@@ -1591,37 +2242,18 @@
       <c r="L18">
         <v>0</v>
       </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-      <c r="R18">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE32397E-FAC9-47C3-882D-4E8AF86978AB}">
   <dimension ref="B1:R18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I3" sqref="B2:R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1643,7 +2275,13 @@
     <col min="18" max="18" width="17.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="R1" s="13"/>
+    </row>
     <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="2"/>
       <c r="C2" s="10" t="s">
@@ -2540,6 +3178,920 @@
         <v>0</v>
       </c>
       <c r="R18" s="6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AD4344-E49F-4CB4-8E6A-362A44079ABA}">
+  <dimension ref="A1:Q17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2"/>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0</v>
+      </c>
+      <c r="N2" s="3">
+        <v>0</v>
+      </c>
+      <c r="O2" s="3">
+        <v>0</v>
+      </c>
+      <c r="P2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3">
+        <v>-1</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <v>-1</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0</v>
+      </c>
+      <c r="N3" s="3">
+        <v>-1</v>
+      </c>
+      <c r="O3" s="3">
+        <v>-1</v>
+      </c>
+      <c r="P3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0</v>
+      </c>
+      <c r="N4" s="3">
+        <v>0</v>
+      </c>
+      <c r="O4" s="3">
+        <v>0</v>
+      </c>
+      <c r="P4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3">
+        <v>-1</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3">
+        <v>-1</v>
+      </c>
+      <c r="K6" s="3">
+        <v>-1</v>
+      </c>
+      <c r="L6" s="3">
+        <v>-1</v>
+      </c>
+      <c r="M6" s="3">
+        <v>-1</v>
+      </c>
+      <c r="N6" s="3">
+        <v>-1</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0</v>
+      </c>
+      <c r="P6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>-1</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0</v>
+      </c>
+      <c r="M7" s="3">
+        <v>1</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0</v>
+      </c>
+      <c r="O7" s="3">
+        <v>0</v>
+      </c>
+      <c r="P7" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>-1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0</v>
+      </c>
+      <c r="M8" s="3">
+        <v>0</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0</v>
+      </c>
+      <c r="P8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3">
+        <v>-1</v>
+      </c>
+      <c r="M9" s="3">
+        <v>0</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0</v>
+      </c>
+      <c r="O9" s="3">
+        <v>0</v>
+      </c>
+      <c r="P9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0</v>
+      </c>
+      <c r="K10" s="3">
+        <v>1</v>
+      </c>
+      <c r="L10" s="3">
+        <v>1</v>
+      </c>
+      <c r="M10" s="3">
+        <v>0</v>
+      </c>
+      <c r="N10" s="3">
+        <v>-1</v>
+      </c>
+      <c r="O10" s="3">
+        <v>1</v>
+      </c>
+      <c r="P10" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+      <c r="J11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3">
+        <v>0</v>
+      </c>
+      <c r="M11" s="3">
+        <v>0</v>
+      </c>
+      <c r="N11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="O11" s="3">
+        <v>1</v>
+      </c>
+      <c r="P11" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3">
+        <v>-1</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0</v>
+      </c>
+      <c r="J12" s="3">
+        <v>-1</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0</v>
+      </c>
+      <c r="L12" s="3">
+        <v>0</v>
+      </c>
+      <c r="M12" s="3">
+        <v>0</v>
+      </c>
+      <c r="N12" s="3">
+        <v>-1</v>
+      </c>
+      <c r="O12" s="3">
+        <v>1</v>
+      </c>
+      <c r="P12" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0</v>
+      </c>
+      <c r="K13" s="3">
+        <v>0</v>
+      </c>
+      <c r="L13" s="3">
+        <v>0</v>
+      </c>
+      <c r="M13" s="3">
+        <v>0</v>
+      </c>
+      <c r="N13" s="3">
+        <v>0</v>
+      </c>
+      <c r="O13" s="3">
+        <v>1</v>
+      </c>
+      <c r="P13" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0</v>
+      </c>
+      <c r="J14" s="3">
+        <v>1</v>
+      </c>
+      <c r="K14" s="3">
+        <v>1</v>
+      </c>
+      <c r="L14" s="3">
+        <v>1</v>
+      </c>
+      <c r="M14" s="3">
+        <v>0</v>
+      </c>
+      <c r="N14" s="3">
+        <v>0</v>
+      </c>
+      <c r="O14" s="3">
+        <v>1</v>
+      </c>
+      <c r="P14" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0</v>
+      </c>
+      <c r="J15" s="3">
+        <v>1</v>
+      </c>
+      <c r="K15" s="3">
+        <v>1</v>
+      </c>
+      <c r="L15" s="3">
+        <v>1</v>
+      </c>
+      <c r="M15" s="3">
+        <v>1</v>
+      </c>
+      <c r="N15" s="3">
+        <v>1</v>
+      </c>
+      <c r="O15" s="3">
+        <v>-1</v>
+      </c>
+      <c r="P15" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0</v>
+      </c>
+      <c r="L16" s="3">
+        <v>0</v>
+      </c>
+      <c r="M16" s="3">
+        <v>0</v>
+      </c>
+      <c r="N16" s="3">
+        <v>0</v>
+      </c>
+      <c r="O16" s="3">
+        <v>0</v>
+      </c>
+      <c r="P16" s="3">
+        <v>-1</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0</v>
+      </c>
+      <c r="I17" s="5">
+        <v>0</v>
+      </c>
+      <c r="J17" s="5">
+        <v>0</v>
+      </c>
+      <c r="K17" s="5">
+        <v>0</v>
+      </c>
+      <c r="L17" s="5">
+        <v>0</v>
+      </c>
+      <c r="M17" s="5">
+        <v>0</v>
+      </c>
+      <c r="N17" s="5">
+        <v>0</v>
+      </c>
+      <c r="O17" s="5">
+        <v>0</v>
+      </c>
+      <c r="P17" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>